<commit_message>
Input mean years 2009,11,13
</commit_message>
<xml_diff>
--- a/src/outputs/3-quintals.xlsx
+++ b/src/outputs/3-quintals.xlsx
@@ -402,16 +402,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>197.24657538</v>
+        <v>199.33698629</v>
       </c>
       <c r="B2" t="n">
-        <v>227.1643835735</v>
+        <v>234.9835616545</v>
       </c>
       <c r="C2" t="n">
-        <v>264.8767122905</v>
+        <v>271.521917789</v>
       </c>
       <c r="D2" t="n">
-        <v>561.8356164740001</v>
+        <v>573.3808218950001</v>
       </c>
       <c r="E2" t="n">
         <v>664</v>
@@ -434,16 +434,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>29</v>
+        <v>29.65</v>
       </c>
       <c r="B3" t="n">
-        <v>73</v>
+        <v>69.8</v>
       </c>
       <c r="C3" t="n">
-        <v>122</v>
+        <v>123.35</v>
       </c>
       <c r="D3" t="n">
-        <v>396</v>
+        <v>348.6</v>
       </c>
       <c r="E3" t="n">
         <v>645</v>
@@ -466,16 +466,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>54.46575342</v>
+        <v>63.71506849</v>
       </c>
       <c r="B4" t="n">
-        <v>149.4246575</v>
+        <v>160.547945237</v>
       </c>
       <c r="C4" t="n">
-        <v>261.8082192</v>
+        <v>269.4465753</v>
       </c>
       <c r="D4" t="n">
-        <v>408.9863014</v>
+        <v>407.2657533870001</v>
       </c>
       <c r="E4" t="n">
         <v>664</v>
@@ -498,16 +498,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>56</v>
+        <v>57.6</v>
       </c>
       <c r="B5" t="n">
-        <v>144</v>
+        <v>145.6</v>
       </c>
       <c r="C5" t="n">
-        <v>252</v>
+        <v>257.2</v>
       </c>
       <c r="D5" t="n">
-        <v>480</v>
+        <v>469.8</v>
       </c>
       <c r="E5" t="n">
         <v>645</v>
@@ -530,16 +530,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>103.424657532</v>
+        <v>103.367123283</v>
       </c>
       <c r="B6" t="n">
-        <v>107.616438359</v>
+        <v>108.350684929</v>
       </c>
       <c r="C6" t="n">
-        <v>108.013698634</v>
+        <v>109.6246575275</v>
       </c>
       <c r="D6" t="n">
-        <v>108.410958909</v>
+        <v>110.898630126</v>
       </c>
       <c r="E6" t="n">
         <v>664</v>
@@ -562,16 +562,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>212</v>
+        <v>208.7</v>
       </c>
       <c r="B7" t="n">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C7" t="n">
-        <v>451</v>
+        <v>446.6</v>
       </c>
       <c r="D7" t="n">
-        <v>904</v>
+        <v>905.2</v>
       </c>
       <c r="E7" t="n">
         <v>645</v>
@@ -594,16 +594,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>63.972602742</v>
+        <v>72.27534247124999</v>
       </c>
       <c r="B8" t="n">
-        <v>126.356164387</v>
+        <v>124.4328767135</v>
       </c>
       <c r="C8" t="n">
-        <v>168.438356149</v>
+        <v>167.338356161</v>
       </c>
       <c r="D8" t="n">
-        <v>201.671232906</v>
+        <v>201.983561631</v>
       </c>
       <c r="E8" t="n">
         <v>664</v>
@@ -626,16 +626,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>60</v>
+        <v>58.15000000000001</v>
       </c>
       <c r="B9" t="n">
-        <v>96</v>
+        <v>91.2</v>
       </c>
       <c r="C9" t="n">
-        <v>130</v>
+        <v>127.15</v>
       </c>
       <c r="D9" t="n">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="E9" t="n">
         <v>645</v>
@@ -658,16 +658,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>456.53424663</v>
+        <v>454.863013717</v>
       </c>
       <c r="B10" t="n">
-        <v>523.328767124</v>
+        <v>522.630137034</v>
       </c>
       <c r="C10" t="n">
-        <v>604.575342527</v>
+        <v>608.6630136935</v>
       </c>
       <c r="D10" t="n">
-        <v>807.2054794519998</v>
+        <v>812.5753424099998</v>
       </c>
       <c r="E10" t="n">
         <v>664</v>
@@ -722,16 +722,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>22.0000000005</v>
+        <v>21.59999999975</v>
       </c>
       <c r="B12" t="n">
-        <v>37.3013698635</v>
+        <v>34.3068493175</v>
       </c>
       <c r="C12" t="n">
-        <v>53.44520547824999</v>
+        <v>52.17123287875</v>
       </c>
       <c r="D12" t="n">
-        <v>106.164383567</v>
+        <v>103.517808213</v>
       </c>
       <c r="E12" t="n">
         <v>664</v>
@@ -757,13 +757,13 @@
         <v>0</v>
       </c>
       <c r="B13" t="n">
-        <v>12.5</v>
+        <v>15.6</v>
       </c>
       <c r="C13" t="n">
-        <v>29.25</v>
+        <v>30.59999999999999</v>
       </c>
       <c r="D13" t="n">
-        <v>34</v>
+        <v>35.8</v>
       </c>
       <c r="E13" t="n">
         <v>645</v>
@@ -786,16 +786,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>328.13698630325</v>
+        <v>327.62876710125</v>
       </c>
       <c r="B14" t="n">
-        <v>351.58904108</v>
+        <v>350.4164383965</v>
       </c>
       <c r="C14" t="n">
-        <v>410.821917774</v>
+        <v>402.0931506715</v>
       </c>
       <c r="D14" t="n">
-        <v>724.8219178389998</v>
+        <v>718.1972601889998</v>
       </c>
       <c r="E14" t="n">
         <v>664</v>
@@ -818,16 +818,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>255.25</v>
+        <v>272.1</v>
       </c>
       <c r="B15" t="n">
-        <v>365</v>
+        <v>367.5999999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>497.75</v>
+        <v>485.9</v>
       </c>
       <c r="D15" t="n">
-        <v>1012</v>
+        <v>981.8000000000003</v>
       </c>
       <c r="E15" t="n">
         <v>645</v>
@@ -874,16 +874,16 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="B17" t="n">
         <v>3</v>
       </c>
       <c r="C17" t="n">
-        <v>9</v>
+        <v>8.4</v>
       </c>
       <c r="D17" t="n">
-        <v>98</v>
+        <v>78.8</v>
       </c>
       <c r="E17" t="n">
         <v>645</v>
@@ -954,16 +954,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>101.219178079</v>
+        <v>102.9315068535</v>
       </c>
       <c r="B20" t="n">
-        <v>120.356164381</v>
+        <v>120.334246518</v>
       </c>
       <c r="C20" t="n">
-        <v>132.1095890505</v>
+        <v>133.460273994</v>
       </c>
       <c r="D20" t="n">
-        <v>276.821917802</v>
+        <v>245.709589081</v>
       </c>
       <c r="E20" t="n">
         <v>664</v>
@@ -986,16 +986,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>174</v>
+        <v>170.8</v>
       </c>
       <c r="B21" t="n">
-        <v>297</v>
+        <v>293.6</v>
       </c>
       <c r="C21" t="n">
-        <v>394</v>
+        <v>390.6</v>
       </c>
       <c r="D21" t="n">
-        <v>600</v>
+        <v>583.5999999999999</v>
       </c>
       <c r="E21" t="n">
         <v>645</v>
@@ -1018,16 +1018,16 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>55.787671235</v>
+        <v>56.84657534</v>
       </c>
       <c r="B22" t="n">
-        <v>92.26027397499999</v>
+        <v>93.41917809</v>
       </c>
       <c r="C22" t="n">
-        <v>122.6712328545</v>
+        <v>123.169863016</v>
       </c>
       <c r="D22" t="n">
-        <v>159.83561647</v>
+        <v>156.027397262</v>
       </c>
       <c r="E22" t="n">
         <v>664</v>
@@ -1050,16 +1050,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>26</v>
+        <v>26.6</v>
       </c>
       <c r="B23" t="n">
-        <v>48</v>
+        <v>46.59999999999999</v>
       </c>
       <c r="C23" t="n">
-        <v>68</v>
+        <v>68.59999999999999</v>
       </c>
       <c r="D23" t="n">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="E23" t="n">
         <v>645</v>

</xml_diff>